<commit_message>
feat: tambah kolom kab_kota di template xlsx
</commit_message>
<xml_diff>
--- a/public/templates/template-data-kelulusan.xlsx
+++ b/public/templates/template-data-kelulusan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen Faidiban\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen Faidiban\Desktop\SMK N 1 Sentani\Lulusan\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8F5A2B-52D3-43F6-BF4B-F7D19F0D51B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20470307-3712-4449-8AA3-0CF2A261FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2130" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>jenjang</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>nomor_ijazah</t>
+  </si>
+  <si>
+    <t>kab_kota</t>
   </si>
 </sst>
 </file>
@@ -385,63 +388,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G2" s="1"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G3" s="1"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>